<commit_message>
Commit with some changes like adding Java docs and restAssured .
</commit_message>
<xml_diff>
--- a/src/test/TestData.xlsx
+++ b/src/test/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cramachandraia\IdeaProjects\com.BestWestern\BWI\src\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA54D634-9BC7-4840-893F-D607EEA09471}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B0A7E6-473E-4E0A-B248-22ABF0B3C13E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{68342319-D8C5-4F40-8690-AEF1A3695D26}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
   <si>
     <t>Destination</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Ustron, Poland</t>
+  </si>
+  <si>
+    <t>USA</t>
   </si>
 </sst>
 </file>
@@ -442,7 +445,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,7 +474,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
         <v>44343</v>
@@ -528,12 +531,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -732,15 +732,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29084BA7-6D1D-42A2-AEEF-F20482B7F85C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E17B436-FB7A-455C-ABC2-EC40D716F5E4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="4fed5f14-e135-4e5e-b4ea-bd6cfacc4996"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c903dae3-5008-45b7-aaaa-6d4304034002"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -765,18 +777,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E17B436-FB7A-455C-ABC2-EC40D716F5E4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29084BA7-6D1D-42A2-AEEF-F20482B7F85C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="4fed5f14-e135-4e5e-b4ea-bd6cfacc4996"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c903dae3-5008-45b7-aaaa-6d4304034002"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Commit with changes like removing white spaces
</commit_message>
<xml_diff>
--- a/src/test/TestData.xlsx
+++ b/src/test/TestData.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cramachandraia\IdeaProjects\com.BestWestern\BWI\src\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B0A7E6-473E-4E0A-B248-22ABF0B3C13E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886B4545-EC95-4093-8937-A8BEE5032312}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{68342319-D8C5-4F40-8690-AEF1A3695D26}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{68342319-D8C5-4F40-8690-AEF1A3695D26}"/>
   </bookViews>
   <sheets>
-    <sheet name="InputData" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="Data" sheetId="4" r:id="rId1"/>
+    <sheet name="InputData" sheetId="3" r:id="rId2"/>
     <sheet name="UpdateInputData" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -404,6 +404,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4B00C99-CF8F-4AB1-8979-ABFE873B0B55}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44275</v>
+      </c>
+      <c r="C2" s="1">
+        <v>44277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44343</v>
+      </c>
+      <c r="C3" s="1">
+        <v>44344</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41B154EB-7756-462E-A692-80D36375F537}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -433,54 +481,6 @@
       </c>
       <c r="C2" s="1">
         <v>44277</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4B00C99-CF8F-4AB1-8979-ABFE873B0B55}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>44275</v>
-      </c>
-      <c r="C2" s="1">
-        <v>44277</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1">
-        <v>44343</v>
-      </c>
-      <c r="C3" s="1">
-        <v>44344</v>
       </c>
     </row>
   </sheetData>
@@ -531,9 +531,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -732,27 +735,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E17B436-FB7A-455C-ABC2-EC40D716F5E4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29084BA7-6D1D-42A2-AEEF-F20482B7F85C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="4fed5f14-e135-4e5e-b4ea-bd6cfacc4996"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c903dae3-5008-45b7-aaaa-6d4304034002"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -777,9 +768,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29084BA7-6D1D-42A2-AEEF-F20482B7F85C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E17B436-FB7A-455C-ABC2-EC40D716F5E4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="4fed5f14-e135-4e5e-b4ea-bd6cfacc4996"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c903dae3-5008-45b7-aaaa-6d4304034002"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>